<commit_message>
إصلاح merge conflict في app.py
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MY APP\PYTHON\Feeder Location\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DEFE691-8CD6-44E2-B039-6200DE220224}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7477E14-E50B-497F-90CE-C564AF761A03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="502" uniqueCount="336">
   <si>
     <t>username</t>
   </si>
@@ -1033,9 +1033,6 @@
   </si>
   <si>
     <t>A.Suliman</t>
-  </si>
-  <si>
-    <t>7pL9dMd</t>
   </si>
 </sst>
 </file>
@@ -1373,7 +1370,7 @@
   <dimension ref="A1:D167"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1427,8 +1424,8 @@
       <c r="A4" t="s">
         <v>335</v>
       </c>
-      <c r="B4" t="s">
-        <v>336</v>
+      <c r="B4">
+        <v>141323</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>

</xml_diff>